<commit_message>
07.20 22:31pm srs, schema written
</commit_message>
<xml_diff>
--- a/doc/db_schema.xlsx
+++ b/doc/db_schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="22590" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22590" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="table_Term" sheetId="3" r:id="rId1"/>
@@ -522,7 +522,7 @@
   <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +656,7 @@
   <dimension ref="A2:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +809,7 @@
   <dimension ref="A2:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
07.28 05:34am edited index, Core, Router, config.xml,,.
</commit_message>
<xml_diff>
--- a/doc/db_schema.xlsx
+++ b/doc/db_schema.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22590" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="22590" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="table_Term" sheetId="3" r:id="rId1"/>
-    <sheet name="table_Member" sheetId="4" r:id="rId2"/>
-    <sheet name="table_Message" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Term" sheetId="3" r:id="rId1"/>
+    <sheet name="Comment" sheetId="6" r:id="rId2"/>
+    <sheet name="Member" sheetId="4" r:id="rId3"/>
+    <sheet name="Message" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="78">
   <si>
     <t>## DB 명세</t>
   </si>
@@ -180,13 +181,94 @@
   </si>
   <si>
     <t>sender's nickname</t>
+  </si>
+  <si>
+    <t>## last edit. 07.23. 2015</t>
+  </si>
+  <si>
+    <t>## Table Name: Comment</t>
+  </si>
+  <si>
+    <t>Example Data</t>
+  </si>
+  <si>
+    <t>극혐</t>
+  </si>
+  <si>
+    <t>심하게 혐오함을 뜻함.</t>
+  </si>
+  <si>
+    <t>그켬</t>
+  </si>
+  <si>
+    <t>극도로 혐오</t>
+  </si>
+  <si>
+    <t>꿀잼</t>
+  </si>
+  <si>
+    <t>매우 재미있다</t>
+  </si>
+  <si>
+    <t>갓-</t>
+  </si>
+  <si>
+    <t>갓</t>
+  </si>
+  <si>
+    <t>칭찬과 존경의 의미를 추가하는 접사</t>
+  </si>
+  <si>
+    <t>흑화</t>
+  </si>
+  <si>
+    <t>흐콰</t>
+  </si>
+  <si>
+    <t>악의 기운에 가까워지다. 악해지게 되다. 혹은 악해지다</t>
+  </si>
+  <si>
+    <t>갈베</t>
+  </si>
+  <si>
+    <t>갈색 일베. 갈색 일베저장소,,. 순서로 파생</t>
+  </si>
+  <si>
+    <t>풀발기</t>
+  </si>
+  <si>
+    <t>빅뱅빠</t>
+  </si>
+  <si>
+    <t>빅뱅과 빠순이의 합성어</t>
+  </si>
+  <si>
+    <t>닭근혜</t>
+  </si>
+  <si>
+    <t>닭과 박근혜의 합성어</t>
+  </si>
+  <si>
+    <t>7시</t>
+  </si>
+  <si>
+    <t>전라도</t>
+  </si>
+  <si>
+    <t>부들부들</t>
+  </si>
+  <si>
+    <t>화가남을 표현하는 의태어</t>
+  </si>
+  <si>
+    <t>full 발기</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +278,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -235,10 +326,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -519,10 +612,471 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="47" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="4">
+        <v>42208</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="4">
+        <v>28148</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1231</v>
+      </c>
+      <c r="J18">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="4">
+        <v>75619</v>
+      </c>
+      <c r="G19">
+        <v>2000</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>22</v>
+      </c>
+      <c r="J19">
+        <v>44.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="4">
+        <v>41943</v>
+      </c>
+      <c r="G20">
+        <v>232</v>
+      </c>
+      <c r="H20">
+        <v>44</v>
+      </c>
+      <c r="I20">
+        <v>5151</v>
+      </c>
+      <c r="J20">
+        <v>67.530900000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="4">
+        <v>42319</v>
+      </c>
+      <c r="G21">
+        <v>7434</v>
+      </c>
+      <c r="H21">
+        <v>3242</v>
+      </c>
+      <c r="I21">
+        <v>23523</v>
+      </c>
+      <c r="J21">
+        <v>67.45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="4">
+        <v>42069</v>
+      </c>
+      <c r="G22">
+        <v>3452</v>
+      </c>
+      <c r="H22">
+        <v>67</v>
+      </c>
+      <c r="I22">
+        <v>456</v>
+      </c>
+      <c r="J22">
+        <v>435.64299999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="4">
+        <v>38667</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>2323</v>
+      </c>
+      <c r="I23">
+        <v>66</v>
+      </c>
+      <c r="J23">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="4">
+        <v>41117</v>
+      </c>
+      <c r="G24">
+        <v>67</v>
+      </c>
+      <c r="H24">
+        <v>43</v>
+      </c>
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="J24">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="4">
+        <v>45971</v>
+      </c>
+      <c r="G25">
+        <v>56</v>
+      </c>
+      <c r="H25">
+        <v>34</v>
+      </c>
+      <c r="I25">
+        <v>56</v>
+      </c>
+      <c r="J25">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="4">
+        <v>82434</v>
+      </c>
+      <c r="G26">
+        <v>1156</v>
+      </c>
+      <c r="H26">
+        <v>1232</v>
+      </c>
+      <c r="I26">
+        <v>12312</v>
+      </c>
+      <c r="J26">
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="4">
+        <v>407376</v>
+      </c>
+      <c r="G27">
+        <v>231</v>
+      </c>
+      <c r="H27">
+        <v>1212</v>
+      </c>
+      <c r="I27">
+        <v>2342</v>
+      </c>
+      <c r="J27">
+        <v>123.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +1100,12 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -651,7 +1210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L10"/>
   <sheetViews>
@@ -804,12 +1363,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +1483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>